<commit_message>
add tx flatness and tor gain test
</commit_message>
<xml_diff>
--- a/bench_setup.xlsx
+++ b/bench_setup.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7290"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HW" sheetId="1" r:id="rId1"/>
     <sheet name="SW" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="setup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -920,6 +920,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>269875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>147955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="711200"/>
+          <a:ext cx="6365875" cy="2103755"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1211,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -2631,13 +2680,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>